<commit_message>
employe document type & bulk create
</commit_message>
<xml_diff>
--- a/public/files/employees/sample-employees.xlsx
+++ b/public/files/employees/sample-employees.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\mini-ecommerce\public\files\customers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\portrans\nozaki\public\files\employees\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51293D31-EE75-45A7-8C18-33753784BC2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C70F69-4E0D-4933-A002-3FD8BFBBAB5E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8AAE6ED2-B5B4-4E8D-B6FF-B27CE4F69FE6}"/>
   </bookViews>
@@ -34,34 +34,159 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>nombre</t>
   </si>
   <si>
-    <t>telefono</t>
-  </si>
-  <si>
-    <t>direccion</t>
-  </si>
-  <si>
-    <t>ciudad</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
     <t>identificacion</t>
+  </si>
+  <si>
+    <t>tipo de documento</t>
+  </si>
+  <si>
+    <t>dirección</t>
+  </si>
+  <si>
+    <t>teléfono</t>
+  </si>
+  <si>
+    <t>cargo</t>
+  </si>
+  <si>
+    <t>rh</t>
+  </si>
+  <si>
+    <t>método de pago</t>
+  </si>
+  <si>
+    <t>banco</t>
+  </si>
+  <si>
+    <t>tipo de cuenta</t>
+  </si>
+  <si>
+    <t>número de cuenta</t>
+  </si>
+  <si>
+    <t>salario</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>fecha de inicio</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>ciudad expedición</t>
+  </si>
+  <si>
+    <t>fecha de nacimiento</t>
+  </si>
+  <si>
+    <t>subsidio</t>
+  </si>
+  <si>
+    <t>tipo de contrato</t>
+  </si>
+  <si>
+    <t>contratación</t>
+  </si>
+  <si>
+    <t>eps</t>
+  </si>
+  <si>
+    <t>cesantias</t>
+  </si>
+  <si>
+    <t>pensiones</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>caja de compensación</t>
+  </si>
+  <si>
+    <t>arl</t>
+  </si>
+  <si>
+    <t>soacha</t>
+  </si>
+  <si>
+    <t>Armando Cristancho</t>
+  </si>
+  <si>
+    <t>actancho@dem.com</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>Carrera demo 123</t>
+  </si>
+  <si>
+    <t>CONDUCTOR</t>
+  </si>
+  <si>
+    <t>O+</t>
+  </si>
+  <si>
+    <t>EFECTIVO</t>
+  </si>
+  <si>
+    <t>BANCOLOMBIA</t>
+  </si>
+  <si>
+    <t>AHORROS</t>
+  </si>
+  <si>
+    <t>MENSUAL</t>
+  </si>
+  <si>
+    <t>EMPLEADO</t>
+  </si>
+  <si>
+    <t>INDEFINIDO</t>
+  </si>
+  <si>
+    <t>NUEVA EPS</t>
+  </si>
+  <si>
+    <t>PORVENIR</t>
+  </si>
+  <si>
+    <t>OPERATIVO</t>
+  </si>
+  <si>
+    <t>COMFACASANARE</t>
+  </si>
+  <si>
+    <t>POSITIVA COMPAÑÍA DE SEGUROS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -84,14 +209,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -404,42 +533,217 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82721DAE-F2ED-455C-8357-F5D4F86BD954}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:AA15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="3.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1076899023</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2">
+        <v>3098997665</v>
+      </c>
+      <c r="J2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2">
+        <v>98888288828</v>
+      </c>
+      <c r="P2">
+        <v>8000000</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" s="3">
+        <v>44252</v>
+      </c>
+      <c r="S2">
+        <v>100000</v>
+      </c>
+      <c r="T2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="G15" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{B8E502A5-3FC4-4560-B29E-F9DA13D9232F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>